<commit_message>
Update template and standards
</commit_message>
<xml_diff>
--- a/docs/SharkTraits-Template.xlsx
+++ b/docs/SharkTraits-Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="33300" yWindow="-2460" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data Entry" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1625" uniqueCount="1583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1626" uniqueCount="1585">
   <si>
     <t>observation_id</t>
   </si>
@@ -4808,7 +4808,13 @@
     <t>Recently Described/Novel Species</t>
   </si>
   <si>
-    <t>Ratio CBD</t>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Coefficient</t>
+  </si>
+  <si>
+    <t>cm PCL</t>
   </si>
 </sst>
 </file>
@@ -5891,10 +5897,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE109"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6430,8 +6436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K769"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A750" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6803,10 +6809,10 @@
         <v>83</v>
       </c>
       <c r="G27" t="s">
-        <v>1564</v>
+        <v>1583</v>
       </c>
       <c r="H27" t="s">
-        <v>1564</v>
+        <v>1583</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>1563</v>
@@ -6893,7 +6899,7 @@
     </row>
     <row r="33" spans="3:11">
       <c r="C33" t="s">
-        <v>85</v>
+        <v>1584</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>88</v>
@@ -6907,7 +6913,7 @@
     </row>
     <row r="34" spans="3:11">
       <c r="C34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>89</v>
@@ -6920,6 +6926,9 @@
       </c>
     </row>
     <row r="35" spans="3:11">
+      <c r="C35" t="s">
+        <v>86</v>
+      </c>
       <c r="F35" s="2" t="s">
         <v>90</v>
       </c>

</xml_diff>

<commit_message>
Update template with generation length
</commit_message>
<xml_diff>
--- a/docs/SharkTraits-Template.xlsx
+++ b/docs/SharkTraits-Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="34600" yWindow="-1820" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data Entry" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="1586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1628" uniqueCount="1587">
   <si>
     <t>observation_id</t>
   </si>
@@ -4818,6 +4818,9 @@
   </si>
   <si>
     <t>Chemical Balance of Development</t>
+  </si>
+  <si>
+    <t>Generation Length</t>
   </si>
 </sst>
 </file>
@@ -6440,7 +6443,7 @@
   <dimension ref="A1:K770"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6630,6 +6633,9 @@
     <row r="12" spans="1:10">
       <c r="C12" s="1" t="s">
         <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1586</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>67</v>

</xml_diff>